<commit_message>
Fix capitalization per #57
</commit_message>
<xml_diff>
--- a/21838-2/bfo-2020-terms.xlsx
+++ b/21838-2/bfo-2020-terms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanr/repos/BFO-2020/21838-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75804BF-8FD1-A94C-953F-06CE9CAF22CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAB5192-DB5A-2147-A84B-F6A90077DE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43660" yWindow="3700" windowWidth="45040" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1533,27 +1533,9 @@
     <t>A material entity is an independent continuant that at all times at which it exists has some portion of matter as continuant part</t>
   </si>
   <si>
-    <t>an object is a material entity which manifests causal unity &amp; is of a type instances of which are maximal relative to the sort of causal unity manifested</t>
-  </si>
-  <si>
-    <t>an object aggregate is a material entity consisting exactly of a plurality (³1) of objects as member parts which together form a unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> a fiat object part b is a material entity which is such that - for all times t, if b exists at t then there is some object c such that b is a proper continuant part of c at t and b is demarcated from the remainder of c by one or more fiat surfaces</t>
-  </si>
-  <si>
     <t>b is a continuant fiat boundary means: b is an immaterial entity that is of zero, one or two dimensions, which is such that there is no time t when b has a spatial region as continuant part at t, and whose location is determined in relation to some material entity</t>
   </si>
   <si>
-    <t>a fiat point is a zero-dimensional continuant fiat boundary that consists of a single point</t>
-  </si>
-  <si>
-    <t>a fiat line is a one-dimensional continuant fiat boundary that is continuous</t>
-  </si>
-  <si>
-    <t>a fiat surface is a two-dimensional continuant fiat boundary that is self-connected</t>
-  </si>
-  <si>
     <t>A spatial region is a continuant entity that is a continuant part of the spatial projection of a portion of spacetime at a given time</t>
   </si>
   <si>
@@ -1569,33 +1551,15 @@
     <t>A three-dimensional spatial region is a whole consisting of a spatial volume together with zero or more spatial volumes and/or spatial regions of lower dimension as parts</t>
   </si>
   <si>
-    <t>a quality is a specifically dependent continuant that, in contrast to roles and dispositions, does not require any further process in order to be realized</t>
-  </si>
-  <si>
-    <t>b is a realizable entity means: b is a specifically dependent continuant that inheres in some independent continuant which is not a spatial region and is of a type some instances of which are realized in processes of a correlated type</t>
-  </si>
-  <si>
-    <t>b is a role means:  b is a realizable entity &amp; b exists because there is some single bearer that is in some special physical, social, or institutional set of circumstances in which this bearer does not have to be &amp; b is not such that, if it ceases to exist, then the physical make-up of the bearer is thereby changed</t>
-  </si>
-  <si>
     <t>b has material basis c at t means: b is a disposition &amp; c is a material entity &amp; there is some d bearer of b &amp; c continuant part of d at t &amp; d has disposition b because c continuant part of d at t</t>
   </si>
   <si>
-    <t>a g-dependent continuant b g-depends on an independent continuant c at t means: there inheres in c an s-dependent continuant which concretizes b at t</t>
-  </si>
-  <si>
     <t>b is carrier of c at t means: c g-depends on b at t</t>
   </si>
   <si>
-    <t>a g-dependent continuant c at t is concretized by an s-dependent continuant or process b when b concretizes c</t>
-  </si>
-  <si>
     <t>An occurrent is an entity that unfolds itself in time or it is the start or end of such an entity or it is a temporal or spatiotemporal region</t>
   </si>
   <si>
-    <t>temporally projects onto is a relation between a spatiotemporal region s and some temporal region which is the temporal extent of s</t>
-  </si>
-  <si>
     <t>p occupies spatiotemporal region s is a relation between an occurrent p and the spatiotemporal region s which is its spatiotemporal extent</t>
   </si>
   <si>
@@ -1617,18 +1581,9 @@
     <t>A one-dimensional temporal region is a temporal region is a whole that has a temporal interval and zero or more temporal intervals and temporal instants as parts</t>
   </si>
   <si>
-    <t>a temporal interval is a one-dimensional temporal region that is continuous, thus without gaps or breaks</t>
-  </si>
-  <si>
-    <t>a temporal instant is a zero-dimensional temporal region that has no proper temporal part</t>
-  </si>
-  <si>
     <t>If o, o' are occurrents and t is the temporal extent of o and t' is the temporal extent of o' then o precedes o’ means: either last instant of o is before first instant of o’ or last instant of o = first instant of o’ and neither o nor o’ are temporal instants</t>
   </si>
   <si>
-    <t>Elucidation: a generically dependent continuant is an entity that exists in virtue of the fact that there is at least one of what may be multiple copies; it is the content or the pattern that the multiple copies share</t>
-  </si>
-  <si>
     <t>b proper continuant part of c at t =Def. b continuant part of c at t &amp; not (c continuant part of b at t)</t>
   </si>
   <si>
@@ -1704,15 +1659,9 @@
     <t>b participates in p at t =Def. p has participant b at t</t>
   </si>
   <si>
-    <t>temporal instant t first instant of temporal region t´ =Def. t precedes all temporal parts of t' other than t</t>
-  </si>
-  <si>
     <t>t has first instant t' =Def. t' first instant of t</t>
   </si>
   <si>
-    <t>temporal instant t last instant of temporal region t´ =Def. all temporal parts of t' other than t precede t</t>
-  </si>
-  <si>
     <t>t has last instant t´ =Def. t´ last instant of t</t>
   </si>
   <si>
@@ -1785,21 +1734,12 @@
     <t>b participates in p at all times =Def. for all times t, b exists at t implies (p has participant b at t)</t>
   </si>
   <si>
-    <t>a g-dependent continuant b g-depends on an independent continuant c at some time =Def. for some time t (there inheres in c an s-dependent continuant which concretizes b at t)</t>
-  </si>
-  <si>
-    <t>a g-dependent continuant b g-depends on an independent continuant c at all times =Def. for all times t, b exists at t implies (there inheres in c an s-dependent continuant which concretizes b at t)</t>
-  </si>
-  <si>
     <t>b is carrier of c at some time =Def. for some time t (c g-depends on b at t)</t>
   </si>
   <si>
     <t>b is carrier of c at all times =Def. for all times t, b exists at t implies (c g-depends on b at t)</t>
   </si>
   <si>
-    <t>a g-dependent continuant c is concretized by an s-dependent continuant or process b at all times =Def. for all times t, b exists at t implies (b concretizes c at t)</t>
-  </si>
-  <si>
     <t>instantiates</t>
   </si>
   <si>
@@ -1815,21 +1755,9 @@
     <t>Planet Earth has continuant part Equator.</t>
   </si>
   <si>
-    <t>an independent continuant c that is not a spatial region occupies spatial region r at t means: every continuant part of c occupies some continuant part of r at t and no continuant part of c occupies any spatial region that is not a continuant part of r at t</t>
-  </si>
-  <si>
-    <t>b realizes c means: there is some material or immaterial entity d &amp; c is a realizable entity that inheres in d &amp; for all t, if b has participant d at t then c exists at t &amp; the type instantiated by b is correlated with the type instantiated by c</t>
-  </si>
-  <si>
     <t>b is a disposition means: b is a realizable entity &amp; b is such that if it ceases to exist, then its bearer is physically changed, &amp; b’s realization occurs when and because this bearer is in some special physical circumstances, &amp; this realization occurs in virtue of the bearer’s physical make-up</t>
   </si>
   <si>
-    <t>an independent continuant c that is not a spatial region occupies spatial region r at some time =Def. for some time t (every continuant part of c occupies some continuant part of r at t and no continuant part of c occupies any spatial region that is not a continuant part of r at t)</t>
-  </si>
-  <si>
-    <t>an independent continuant c that is not a spatial region occupies spatial region r at all times =Def. for all times t, b exists at t implies (every continuant part of c occupies some continuant part of r at t and no continuant part of c occupies any spatial region that is not a continuant part of r at t)</t>
-  </si>
-  <si>
     <t>The temporal region occupied by the second half of the match is preceded by the temporal region occupied by the first half of the match.</t>
   </si>
   <si>
@@ -1866,15 +1794,6 @@
     <t>b proper continuant part of c at some time =Def. for some time t (b continuant part of c at t &amp; not (c continuant part of b at t))</t>
   </si>
   <si>
-    <t>an s-dependent continuant or process b concretizes a g-dependent continuant c at some time =Def. for some time t (c is the pattern or content which b shares at t with actual or potential copies)</t>
-  </si>
-  <si>
-    <t>an s-dependent continuant or process b concretizes a g-dependent continuant c at all times =Def. for all times t, b exists at t implies (c is the pattern or content which b shares at t with actual or potential copies)</t>
-  </si>
-  <si>
-    <t>a g-dependent continuant c is concretized at some time by an s-dependent continuant or process b =Def. for some time t, b concretizes c at t</t>
-  </si>
-  <si>
     <t>p has participant c at some time =Def. for some time t (p is a process, c is a continuant, and c participates in p some way at t)</t>
   </si>
   <si>
@@ -1950,15 +1869,96 @@
     <t>location of</t>
   </si>
   <si>
-    <t>an s-dependent continuant or process b concretizes a g-dependent continuant c at all times means: for all times t, b exists at t implies that: 
+    <t>p is a process means: p is an occurrent that has some temporal proper part and for some time t, p has some material entity as participant at t</t>
+  </si>
+  <si>
+    <t>Term/Relational Expression</t>
+  </si>
+  <si>
+    <t>An object is a material entity which manifests causal unity &amp; is of a type instances of which are maximal relative to the sort of causal unity manifested</t>
+  </si>
+  <si>
+    <t>An object aggregate is a material entity consisting exactly of a plurality (³1) of objects as member parts which together form a unit</t>
+  </si>
+  <si>
+    <t>A fiat object part b is a material entity which is such that - for all times t, if b exists at t then there is some object c such that b is a proper continuant part of c at t and b is demarcated from the remainder of c by one or more fiat surfaces</t>
+  </si>
+  <si>
+    <t>A fiat point is a zero-dimensional continuant fiat boundary that consists of a single point</t>
+  </si>
+  <si>
+    <t>A fiat line is a one-dimensional continuant fiat boundary that is continuous</t>
+  </si>
+  <si>
+    <t>A fiat surface is a two-dimensional continuant fiat boundary that is self-connected</t>
+  </si>
+  <si>
+    <t>An independent continuant c that is not a spatial region occupies spatial region r at t means: every continuant part of c occupies some continuant part of r at t and no continuant part of c occupies any spatial region that is not a continuant part of r at t</t>
+  </si>
+  <si>
+    <t>A quality is a specifically dependent continuant that, in contrast to roles and dispositions, does not require any further process in order to be realized</t>
+  </si>
+  <si>
+    <t>A is a realizable entity means: b is a specifically dependent continuant that inheres in some independent continuant which is not a spatial region and is of a type some instances of which are realized in processes of a correlated type</t>
+  </si>
+  <si>
+    <t>A realizes c means: there is some material or immaterial entity d &amp; c is a realizable entity that inheres in d &amp; for all t, if b has participant d at t then c exists at t &amp; the type instantiated by b is correlated with the type instantiated by c</t>
+  </si>
+  <si>
+    <t>A is a role means:  b is a realizable entity &amp; b exists because there is some single bearer that is in some special physical, social, or institutional set of circumstances in which this bearer does not have to be &amp; b is not such that, if it ceases to exist, then the physical make-up of the bearer is thereby changed</t>
+  </si>
+  <si>
+    <t>A generically dependent continuant is an entity that exists in virtue of the fact that there is at least one of what may be multiple copies; it is the content or the pattern that the multiple copies share</t>
+  </si>
+  <si>
+    <t>A g-dependent continuant b g-depends on an independent continuant c at t means: there inheres in c an s-dependent continuant which concretizes b at t</t>
+  </si>
+  <si>
+    <t>An s-dependent continuant or process b concretizes a g-dependent continuant c at all times means: for all times t, b exists at t implies that: 
 if b instance of s-dependent continuant at t, then c is the pattern or content which b shares at t with actual or potential copies of b
 &amp; if b instance of process, then b unfolds according to the pattern or content which b shares at t with actual or potential copies and is sufficient to enable another concretization of c to come into existence. [207-BFO]</t>
   </si>
   <si>
-    <t>p is a process means: p is an occurrent that has some temporal proper part and for some time t, p has some material entity as participant at t</t>
-  </si>
-  <si>
-    <t>Term/Relational Expression</t>
+    <t>A g-dependent continuant c at t is concretized by an s-dependent continuant or process b when b concretizes c</t>
+  </si>
+  <si>
+    <t>Temporally projects onto is a relation between a spatiotemporal region s and some temporal region which is the temporal extent of s</t>
+  </si>
+  <si>
+    <t>A temporal interval is a one-dimensional temporal region that is continuous, thus without gaps or breaks</t>
+  </si>
+  <si>
+    <t>A temporal instant is a zero-dimensional temporal region that has no proper temporal part</t>
+  </si>
+  <si>
+    <t>Temporal instant t first instant of temporal region t´ =Def. t precedes all temporal parts of t' other than t</t>
+  </si>
+  <si>
+    <t>Temporal instant t last instant of temporal region t´ =Def. all temporal parts of t' other than t precede t</t>
+  </si>
+  <si>
+    <t>An independent continuant c that is not a spatial region occupies spatial region r at some time =Def. for some time t (every continuant part of c occupies some continuant part of r at t and no continuant part of c occupies any spatial region that is not a continuant part of r at t)</t>
+  </si>
+  <si>
+    <t>An independent continuant c that is not a spatial region occupies spatial region r at all times =Def. for all times t, b exists at t implies (every continuant part of c occupies some continuant part of r at t and no continuant part of c occupies any spatial region that is not a continuant part of r at t)</t>
+  </si>
+  <si>
+    <t>A g-dependent continuant c is concretized by an s-dependent continuant or process b at all times =Def. for all times t, b exists at t implies (b concretizes c at t)</t>
+  </si>
+  <si>
+    <t>A g-dependent continuant c is concretized at some time by an s-dependent continuant or process b =Def. for some time t, b concretizes c at t</t>
+  </si>
+  <si>
+    <t>An s-dependent continuant or process b concretizes a g-dependent continuant c at all times =Def. for all times t, b exists at t implies (c is the pattern or content which b shares at t with actual or potential copies)</t>
+  </si>
+  <si>
+    <t>An s-dependent continuant or process b concretizes a g-dependent continuant c at some time =Def. for some time t (c is the pattern or content which b shares at t with actual or potential copies)</t>
+  </si>
+  <si>
+    <t>A g-dependent continuant b g-depends on an independent continuant c at all times =Def. for all times t, b exists at t implies (there inheres in c an s-dependent continuant which concretizes b at t)</t>
+  </si>
+  <si>
+    <t>A g-dependent continuant b g-depends on an independent continuant c at some time =Def. for some time t (there inheres in c an s-dependent continuant which concretizes b at t)</t>
   </si>
 </sst>
 </file>
@@ -2398,8 +2398,8 @@
   <dimension ref="A1:K123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="194" zoomScaleNormal="194" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>601</v>
+        <v>573</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>
@@ -2513,7 +2513,7 @@
         <v>14</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>549</v>
+        <v>529</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>129</v>
@@ -2550,7 +2550,7 @@
         <v>256</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>586</v>
+        <v>559</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>454</v>
@@ -2573,17 +2573,17 @@
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>551</v>
+        <v>531</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>590</v>
+        <v>563</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="5" t="s">
-        <v>589</v>
+        <v>562</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>553</v>
+        <v>533</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>22</v>
@@ -2592,7 +2592,7 @@
         <v>22</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>552</v>
+        <v>532</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.2">
@@ -2646,10 +2646,10 @@
         <v>261</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>587</v>
+        <v>560</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>492</v>
+        <v>477</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>28</v>
@@ -2669,10 +2669,10 @@
         <v>262</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>588</v>
+        <v>561</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>29</v>
@@ -2695,7 +2695,7 @@
         <v>264</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>30</v>
@@ -2718,7 +2718,7 @@
         <v>266</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>31</v>
@@ -2767,7 +2767,7 @@
         <v>34</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>33</v>
@@ -2787,7 +2787,7 @@
         <v>271</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>39</v>
@@ -2813,7 +2813,7 @@
         <v>273</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>497</v>
+        <v>482</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>40</v>
@@ -2847,7 +2847,7 @@
         <v>44</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>460</v>
+        <v>574</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>42</v>
@@ -2864,13 +2864,13 @@
         <v>276</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>591</v>
+        <v>564</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>593</v>
+        <v>566</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>44</v>
@@ -2887,10 +2887,10 @@
         <v>277</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>592</v>
+        <v>565</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>499</v>
+        <v>484</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>46</v>
@@ -2913,10 +2913,10 @@
         <v>45</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>461</v>
+        <v>575</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>594</v>
+        <v>567</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>146</v>
@@ -2925,7 +2925,7 @@
         <v>47</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>595</v>
+        <v>568</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.2">
@@ -2936,7 +2936,7 @@
         <v>280</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>462</v>
+        <v>576</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>48</v>
@@ -2953,7 +2953,7 @@
         <v>282</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>500</v>
+        <v>485</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>49</v>
@@ -2970,7 +2970,7 @@
         <v>284</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>50</v>
@@ -2987,7 +2987,7 @@
         <v>286</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>464</v>
+        <v>577</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>51</v>
@@ -3004,7 +3004,7 @@
         <v>287</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>465</v>
+        <v>578</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>52</v>
@@ -3021,7 +3021,7 @@
         <v>288</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>466</v>
+        <v>579</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>53</v>
@@ -3038,10 +3038,10 @@
         <v>299</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>564</v>
+        <v>540</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>565</v>
+        <v>541</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>157</v>
@@ -3055,7 +3055,7 @@
         <v>60</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>54</v>
@@ -3072,7 +3072,7 @@
         <v>300</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>55</v>
@@ -3089,7 +3089,7 @@
         <v>301</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>56</v>
@@ -3106,7 +3106,7 @@
         <v>302</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>57</v>
@@ -3123,7 +3123,7 @@
         <v>303</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>58</v>
@@ -3137,10 +3137,10 @@
         <v>366</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>596</v>
+        <v>569</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>554</v>
+        <v>580</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>61</v>
@@ -3163,10 +3163,10 @@
         <v>367</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>597</v>
+        <v>570</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>501</v>
+        <v>486</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>63</v>
@@ -3186,10 +3186,10 @@
         <v>368</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>598</v>
+        <v>571</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>502</v>
+        <v>487</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>64</v>
@@ -3212,7 +3212,7 @@
         <v>34</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>503</v>
+        <v>488</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>65</v>
@@ -3232,7 +3232,7 @@
         <v>289</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>504</v>
+        <v>489</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>67</v>
@@ -3255,7 +3255,7 @@
         <v>290</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>505</v>
+        <v>490</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>68</v>
@@ -3278,7 +3278,7 @@
         <v>304</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>472</v>
+        <v>581</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>69</v>
@@ -3295,7 +3295,7 @@
         <v>291</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>506</v>
+        <v>491</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>70</v>
@@ -3312,7 +3312,7 @@
         <v>73</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>473</v>
+        <v>582</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>71</v>
@@ -3329,7 +3329,7 @@
         <v>305</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>555</v>
+        <v>583</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>74</v>
@@ -3352,10 +3352,10 @@
         <v>292</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>507</v>
+        <v>492</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>563</v>
+        <v>539</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>73</v>
@@ -3375,7 +3375,7 @@
         <v>306</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>474</v>
+        <v>584</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>75</v>
@@ -3395,7 +3395,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>556</v>
+        <v>534</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>78</v>
@@ -3417,10 +3417,10 @@
         <v>379</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>576</v>
+        <v>549</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>213</v>
@@ -3440,10 +3440,10 @@
         <v>380</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>577</v>
+        <v>550</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>566</v>
+        <v>542</v>
       </c>
       <c r="E50" s="10" t="s">
         <v>214</v>
@@ -3466,7 +3466,7 @@
         <v>86</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>491</v>
+        <v>585</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>83</v>
@@ -3480,7 +3480,7 @@
     </row>
     <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="C52" s="7" t="s">
-        <v>476</v>
+        <v>586</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>175</v>
@@ -3491,7 +3491,7 @@
         <v>382</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>578</v>
+        <v>551</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>85</v>
@@ -3511,13 +3511,13 @@
         <v>383</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>579</v>
+        <v>552</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>561</v>
+        <v>537</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>59</v>
@@ -3534,10 +3534,10 @@
         <v>384</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>580</v>
+        <v>553</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>88</v>
@@ -3557,10 +3557,10 @@
         <v>385</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>581</v>
+        <v>554</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>478</v>
+        <v>588</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>89</v>
@@ -3583,7 +3583,7 @@
         <v>25</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>90</v>
@@ -3600,10 +3600,10 @@
         <v>307</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>567</v>
+        <v>543</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>562</v>
+        <v>538</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>25</v>
@@ -3623,7 +3623,7 @@
         <v>308</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>91</v>
@@ -3646,7 +3646,7 @@
         <v>309</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>509</v>
+        <v>494</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>215</v>
@@ -3669,7 +3669,7 @@
         <v>310</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>510</v>
+        <v>495</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>216</v>
@@ -3692,7 +3692,7 @@
         <v>311</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>480</v>
+        <v>589</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>93</v>
@@ -3712,10 +3712,10 @@
         <v>392</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>582</v>
+        <v>555</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>568</v>
+        <v>544</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>94</v>
@@ -3738,10 +3738,10 @@
         <v>312</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>569</v>
+        <v>545</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>95</v>
@@ -3761,7 +3761,7 @@
         <v>313</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>511</v>
+        <v>496</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>96</v>
@@ -3784,7 +3784,7 @@
         <v>293</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>512</v>
+        <v>497</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>98</v>
@@ -3807,7 +3807,7 @@
         <v>314</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>513</v>
+        <v>498</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>99</v>
@@ -3830,7 +3830,7 @@
         <v>72</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>600</v>
+        <v>572</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>100</v>
@@ -3847,7 +3847,7 @@
         <v>102</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>101</v>
@@ -3864,7 +3864,7 @@
         <v>294</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>103</v>
@@ -3887,7 +3887,7 @@
         <v>295</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>514</v>
+        <v>499</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>104</v>
@@ -3910,7 +3910,7 @@
         <v>296</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>515</v>
+        <v>500</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>105</v>
@@ -3924,10 +3924,10 @@
         <v>402</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>583</v>
+        <v>556</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>585</v>
+        <v>558</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>107</v>
@@ -3947,10 +3947,10 @@
         <v>403</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>584</v>
+        <v>557</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>516</v>
+        <v>501</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>108</v>
@@ -3973,7 +3973,7 @@
         <v>92</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>110</v>
@@ -3993,7 +3993,7 @@
         <v>20</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>111</v>
@@ -4010,7 +4010,7 @@
         <v>315</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>112</v>
@@ -4027,7 +4027,7 @@
         <v>316</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>113</v>
@@ -4044,7 +4044,7 @@
         <v>297</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>488</v>
+        <v>590</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>114</v>
@@ -4064,7 +4064,7 @@
         <v>117</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>489</v>
+        <v>591</v>
       </c>
       <c r="E80" s="7" t="s">
         <v>116</v>
@@ -4081,7 +4081,7 @@
         <v>317</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>517</v>
+        <v>592</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>118</v>
@@ -4104,7 +4104,7 @@
         <v>318</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>119</v>
@@ -4128,7 +4128,7 @@
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="7" t="s">
-        <v>519</v>
+        <v>593</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>120</v>
@@ -4151,7 +4151,7 @@
         <v>320</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>520</v>
+        <v>503</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>121</v>
@@ -4174,7 +4174,7 @@
         <v>321</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>122</v>
@@ -4203,10 +4203,10 @@
         <v>298</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>560</v>
+        <v>536</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>559</v>
+        <v>535</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>25</v>
@@ -4234,7 +4234,7 @@
         <v>322</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>521</v>
+        <v>504</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>127</v>
@@ -4251,7 +4251,7 @@
         <v>323</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>522</v>
+        <v>505</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>128</v>
@@ -4268,7 +4268,7 @@
         <v>324</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>523</v>
+        <v>506</v>
       </c>
       <c r="I90" s="5" t="s">
         <v>218</v>
@@ -4282,7 +4282,7 @@
         <v>325</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
       <c r="I91" s="5" t="s">
         <v>219</v>
@@ -4296,7 +4296,7 @@
         <v>326</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>570</v>
+        <v>546</v>
       </c>
       <c r="I92" s="5" t="s">
         <v>220</v>
@@ -4310,7 +4310,7 @@
         <v>327</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>525</v>
+        <v>508</v>
       </c>
       <c r="I93" s="5" t="s">
         <v>221</v>
@@ -4324,7 +4324,7 @@
         <v>328</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
       <c r="I94" s="5" t="s">
         <v>222</v>
@@ -4338,7 +4338,7 @@
         <v>329</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>527</v>
+        <v>510</v>
       </c>
       <c r="I95" s="5" t="s">
         <v>223</v>
@@ -4352,7 +4352,7 @@
         <v>330</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>528</v>
+        <v>511</v>
       </c>
       <c r="I96" s="5" t="s">
         <v>224</v>
@@ -4366,7 +4366,7 @@
         <v>331</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>529</v>
+        <v>512</v>
       </c>
       <c r="I97" s="5" t="s">
         <v>225</v>
@@ -4380,7 +4380,7 @@
         <v>332</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>530</v>
+        <v>513</v>
       </c>
       <c r="I98" s="5" t="s">
         <v>226</v>
@@ -4394,7 +4394,7 @@
         <v>333</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>531</v>
+        <v>514</v>
       </c>
       <c r="I99" s="5" t="s">
         <v>227</v>
@@ -4408,7 +4408,7 @@
         <v>334</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>557</v>
+        <v>594</v>
       </c>
       <c r="I100" s="5" t="s">
         <v>228</v>
@@ -4422,7 +4422,7 @@
         <v>335</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>558</v>
+        <v>595</v>
       </c>
       <c r="I101" s="5" t="s">
         <v>229</v>
@@ -4436,7 +4436,7 @@
         <v>336</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>532</v>
+        <v>515</v>
       </c>
       <c r="I102" s="5" t="s">
         <v>230</v>
@@ -4450,7 +4450,7 @@
         <v>337</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>533</v>
+        <v>516</v>
       </c>
       <c r="I103" s="5" t="s">
         <v>231</v>
@@ -4464,7 +4464,7 @@
         <v>338</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>534</v>
+        <v>517</v>
       </c>
       <c r="I104" s="5" t="s">
         <v>232</v>
@@ -4478,7 +4478,7 @@
         <v>339</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>535</v>
+        <v>518</v>
       </c>
       <c r="I105" s="5" t="s">
         <v>233</v>
@@ -4492,7 +4492,7 @@
         <v>340</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>536</v>
+        <v>519</v>
       </c>
       <c r="I106" s="5" t="s">
         <v>234</v>
@@ -4506,7 +4506,7 @@
         <v>341</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>537</v>
+        <v>520</v>
       </c>
       <c r="I107" s="5" t="s">
         <v>235</v>
@@ -4520,7 +4520,7 @@
         <v>342</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>538</v>
+        <v>521</v>
       </c>
       <c r="I108" s="5" t="s">
         <v>236</v>
@@ -4534,7 +4534,7 @@
         <v>343</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>539</v>
+        <v>522</v>
       </c>
       <c r="I109" s="5" t="s">
         <v>237</v>
@@ -4548,7 +4548,7 @@
         <v>344</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
       <c r="I110" s="5" t="s">
         <v>238</v>
@@ -4562,7 +4562,7 @@
         <v>345</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>541</v>
+        <v>524</v>
       </c>
       <c r="I111" s="5" t="s">
         <v>239</v>
@@ -4576,7 +4576,7 @@
         <v>346</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>574</v>
+        <v>547</v>
       </c>
       <c r="I112" s="5" t="s">
         <v>240</v>
@@ -4590,7 +4590,7 @@
         <v>347</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>575</v>
+        <v>548</v>
       </c>
       <c r="I113" s="5" t="s">
         <v>241</v>
@@ -4604,7 +4604,7 @@
         <v>348</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>542</v>
+        <v>525</v>
       </c>
       <c r="I114" s="5" t="s">
         <v>242</v>
@@ -4618,7 +4618,7 @@
         <v>349</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>543</v>
+        <v>526</v>
       </c>
       <c r="I115" s="5" t="s">
         <v>243</v>
@@ -4632,7 +4632,7 @@
         <v>350</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>544</v>
+        <v>601</v>
       </c>
       <c r="H116" s="5" t="s">
         <v>84</v>
@@ -4649,7 +4649,7 @@
         <v>351</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>545</v>
+        <v>600</v>
       </c>
       <c r="H117" s="5" t="s">
         <v>84</v>
@@ -4666,7 +4666,7 @@
         <v>352</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>546</v>
+        <v>527</v>
       </c>
       <c r="I118" s="5" t="s">
         <v>246</v>
@@ -4680,7 +4680,7 @@
         <v>353</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>547</v>
+        <v>528</v>
       </c>
       <c r="I119" s="5" t="s">
         <v>247</v>
@@ -4694,7 +4694,7 @@
         <v>354</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>571</v>
+        <v>599</v>
       </c>
       <c r="I120" s="5" t="s">
         <v>248</v>
@@ -4708,7 +4708,7 @@
         <v>355</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>572</v>
+        <v>598</v>
       </c>
       <c r="I121" s="5" t="s">
         <v>249</v>
@@ -4722,7 +4722,7 @@
         <v>356</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>573</v>
+        <v>597</v>
       </c>
       <c r="I122" s="5" t="s">
         <v>250</v>
@@ -4736,7 +4736,7 @@
         <v>357</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>548</v>
+        <v>596</v>
       </c>
       <c r="I123" s="5" t="s">
         <v>251</v>

</xml_diff>

<commit_message>
Get rid of some invisible spaces. Curse you Microsoft.
</commit_message>
<xml_diff>
--- a/21838-2/bfo-2020-terms.xlsx
+++ b/21838-2/bfo-2020-terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanr/repos/BFO-2020/21838-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAB5192-DB5A-2147-A84B-F6A90077DE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25BC31C-0018-2748-BFBF-B0991E3716EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43660" yWindow="3700" windowWidth="45040" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -297,9 +297,6 @@
     <t xml:space="preserve">The sum of patterns of ink on the pages of this copy of War and Peace concretizes the novel written by Tolstoy. </t>
   </si>
   <si>
-    <t xml:space="preserve">This set of dots and dashes concretizes this Morse code message.  </t>
-  </si>
-  <si>
     <t>As for A.1.2.66, A.1.2.67, A.1.2.70, A.1.2.73, A.1.2.75–A.1.2.78.</t>
   </si>
   <si>
@@ -658,9 +655,6 @@
   </si>
   <si>
     <t>[221-BFO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.1.2.2  </t>
   </si>
   <si>
     <r>
@@ -760,21 +754,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">The material basis of the disposition of the rocket to move is its engine and the fuel supply, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>As for</t>
     </r>
     <r>
@@ -909,15 +888,9 @@
     <t>[259-BFO]</t>
   </si>
   <si>
-    <t>A.1.2.3 </t>
-  </si>
-  <si>
     <t xml:space="preserve">instance of </t>
   </si>
   <si>
-    <t>A.1.2.4 </t>
-  </si>
-  <si>
     <t>exists at</t>
   </si>
   <si>
@@ -1776,9 +1749,6 @@
     <t>b is a site means: b is a three-dimensional immaterial entity whose boundaries either (1) (partially or wholly) coincide with the boundaries of one or more material entities or (2) have locations determined in relation to some material entity</t>
   </si>
   <si>
-    <t>A hole in a portion of cheese, a rabbit hole, the Grand Canyon, the Piazza San Marco, the kangaroo-joey-containing hole of a kangaroo pouch, your left nostril (a fiat part – the opening – of your left nasal cavity), the  lumen of your gut, the hold of a ship, the interior of the trunk of your car, a hole in an engineered floor joist.  An air traffic control region of type A is determined in terms of elevation above mean sea level of its lower and upper boundaries.</t>
-  </si>
-  <si>
     <t>b material basis of c at t =Def. c has material basis b at t</t>
   </si>
   <si>
@@ -1903,9 +1873,6 @@
   </si>
   <si>
     <t>A realizes c means: there is some material or immaterial entity d &amp; c is a realizable entity that inheres in d &amp; for all t, if b has participant d at t then c exists at t &amp; the type instantiated by b is correlated with the type instantiated by c</t>
-  </si>
-  <si>
-    <t>A is a role means:  b is a realizable entity &amp; b exists because there is some single bearer that is in some special physical, social, or institutional set of circumstances in which this bearer does not have to be &amp; b is not such that, if it ceases to exist, then the physical make-up of the bearer is thereby changed</t>
   </si>
   <si>
     <t>A generically dependent continuant is an entity that exists in virtue of the fact that there is at least one of what may be multiple copies; it is the content or the pattern that the multiple copies share</t>
@@ -1959,6 +1926,27 @@
   </si>
   <si>
     <t>A g-dependent continuant b g-depends on an independent continuant c at some time =Def. for some time t (there inheres in c an s-dependent continuant which concretizes b at t)</t>
+  </si>
+  <si>
+    <t>A hole in a portion of cheese, a rabbit hole, the Grand Canyon, the Piazza San Marco, the kangaroo-joey-containing hole of a kangaroo pouch, your left nostril (a fiat part – the opening – of your left nasal cavity), the lumen of your gut, the hold of a ship, the interior of the trunk of your car, a hole in an engineered floor joist. An air traffic control region of type A is determined in terms of elevation above mean sea level of its lower and upper boundaries.</t>
+  </si>
+  <si>
+    <t>A is a role means: b is a realizable entity &amp; b exists because there is some single bearer that is in some special physical, social, or institutional set of circumstances in which this bearer does not have to be &amp; b is not such that, if it ceases to exist, then the physical make-up of the bearer is thereby changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The material basis of the disposition of the rocket to move is its engine and the fuel supply, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This set of dots and dashes concretizes this Morse code message. </t>
+  </si>
+  <si>
+    <t>A.1.2.2</t>
+  </si>
+  <si>
+    <t>A.1.2.3</t>
+  </si>
+  <si>
+    <t>A.1.2.4</t>
   </si>
 </sst>
 </file>
@@ -2399,7 +2387,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="194" zoomScaleNormal="194" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2423,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>
@@ -2464,7 +2452,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>11</v>
@@ -2472,13 +2460,13 @@
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>210</v>
+        <v>599</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>15</v>
@@ -2495,13 +2483,13 @@
     </row>
     <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>252</v>
+        <v>600</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>17</v>
@@ -2513,10 +2501,10 @@
         <v>14</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>19</v>
@@ -2524,13 +2512,13 @@
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>254</v>
+        <v>601</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>21</v>
@@ -2542,18 +2530,18 @@
         <v>20</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>23</v>
@@ -2565,7 +2553,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>24</v>
@@ -2573,17 +2561,17 @@
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="5" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>22</v>
@@ -2592,18 +2580,18 @@
         <v>22</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>26</v>
@@ -2615,18 +2603,18 @@
         <v>25</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>27</v>
@@ -2638,18 +2626,18 @@
         <v>25</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>28</v>
@@ -2661,18 +2649,18 @@
         <v>22</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>29</v>
@@ -2684,18 +2672,18 @@
         <v>22</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>30</v>
@@ -2707,18 +2695,18 @@
         <v>25</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>31</v>
@@ -2730,35 +2718,35 @@
         <v>25</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>36</v>
@@ -2767,13 +2755,13 @@
         <v>34</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>37</v>
@@ -2781,13 +2769,13 @@
     </row>
     <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>39</v>
@@ -2802,58 +2790,58 @@
         <v>38</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>40</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>41</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>42</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>43</v>
@@ -2861,16 +2849,16 @@
     </row>
     <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>44</v>
@@ -2879,18 +2867,18 @@
         <v>45</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>46</v>
@@ -2902,245 +2890,245 @@
         <v>44</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="90" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>47</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>48</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>49</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>50</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>51</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>52</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>53</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>541</v>
+        <v>595</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>54</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>55</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>56</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>57</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>58</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>61</v>
@@ -3152,7 +3140,7 @@
         <v>60</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J35" s="7" t="s">
         <v>62</v>
@@ -3160,13 +3148,13 @@
     </row>
     <row r="36" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>63</v>
@@ -3178,18 +3166,18 @@
         <v>59</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>64</v>
@@ -3201,24 +3189,24 @@
         <v>59</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="105" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>65</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J38" s="8" t="s">
         <v>66</v>
@@ -3226,13 +3214,13 @@
     </row>
     <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>67</v>
@@ -3244,18 +3232,18 @@
         <v>59</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>68</v>
@@ -3267,69 +3255,69 @@
         <v>34</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>69</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>70</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>71</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>74</v>
@@ -3341,21 +3329,21 @@
         <v>73</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>73</v>
@@ -3364,18 +3352,18 @@
         <v>72</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>75</v>
@@ -3384,18 +3372,18 @@
         <v>76</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>78</v>
@@ -3404,7 +3392,7 @@
         <v>77</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -3414,16 +3402,16 @@
     </row>
     <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>80</v>
@@ -3432,21 +3420,21 @@
         <v>81</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>214</v>
+        <v>597</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>59</v>
@@ -3455,18 +3443,18 @@
         <v>80</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="90" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>86</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>83</v>
@@ -3475,23 +3463,23 @@
         <v>82</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="C52" s="7" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>85</v>
@@ -3508,16 +3496,16 @@
     </row>
     <row r="54" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>59</v>
@@ -3526,18 +3514,18 @@
         <v>86</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="150" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>88</v>
@@ -3549,21 +3537,21 @@
         <v>86</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>89</v>
+        <v>598</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>87</v>
@@ -3572,38 +3560,38 @@
         <v>86</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="165" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>25</v>
@@ -3612,21 +3600,21 @@
         <v>25</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>25</v>
@@ -3635,21 +3623,21 @@
         <v>25</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>25</v>
@@ -3658,21 +3646,21 @@
         <v>25</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>25</v>
@@ -3681,503 +3669,503 @@
         <v>25</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>60</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="135" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>72</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>72</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>72</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J75" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="E79" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="J79" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="J79" s="7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>20</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="7" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>20</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="120" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>25</v>
@@ -4186,27 +4174,27 @@
         <v>25</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J85" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="K85" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="K85" s="7" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>25</v>
@@ -4215,531 +4203,531 @@
         <v>25</v>
       </c>
       <c r="I86" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I88" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="I92" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="I93" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="I95" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="90" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="I97" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="I98" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="I99" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="I100" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="105" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="I101" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="90" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="I102" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="90" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="I103" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="I104" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="I105" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="90" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="I106" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="90" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="I107" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="I108" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="I109" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="I110" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="I112" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="I113" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="I114" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="I115" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="H116" s="5" t="s">
         <v>84</v>
       </c>
       <c r="I116" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="H117" s="5" t="s">
         <v>84</v>
       </c>
       <c r="I117" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="I118" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="I119" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="I120" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="I121" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="I122" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="I123" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix text definition of relational quality
</commit_message>
<xml_diff>
--- a/21838-2/bfo-2020-terms.xlsx
+++ b/21838-2/bfo-2020-terms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanr/repos/BFO-2020/21838-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keil_jn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAB5192-DB5A-2147-A84B-F6A90077DE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7691A53-9F21-4D33-9CAD-E1309ABB5A63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43660" yWindow="3700" windowWidth="45040" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1626,9 +1626,6 @@
     <t>b bearer of c =Def. c inheres in b</t>
   </si>
   <si>
-    <t>b is a relational quality =Def. b is a quality and there exists c and d such that b and c are not identical, &amp; b s-depends on c &amp; b s-depends on d</t>
-  </si>
-  <si>
     <t>b has realization c =Def. c realizes b</t>
   </si>
   <si>
@@ -1959,6 +1956,9 @@
   </si>
   <si>
     <t>A g-dependent continuant b g-depends on an independent continuant c at some time =Def. for some time t (there inheres in c an s-dependent continuant which concretizes b at t)</t>
+  </si>
+  <si>
+    <t>b is a relational quality =Def. b is a quality and there exists c and d such that c and d are not identical, &amp; b s-depends on c &amp; b s-depends on d</t>
   </si>
 </sst>
 </file>
@@ -2083,7 +2083,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2099,7 +2099,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2398,32 +2398,32 @@
   <dimension ref="A1:K123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="194" zoomScaleNormal="194" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="5"/>
     <col min="2" max="2" width="23" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="46.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="24.83203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="31.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="46.625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="24.875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.375" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" style="5" customWidth="1"/>
     <col min="11" max="11" width="22" style="5" customWidth="1"/>
     <col min="12" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>
@@ -2453,7 +2453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>210</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>252</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>14</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>129</v>
@@ -2522,7 +2522,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>254</v>
       </c>
@@ -2545,12 +2545,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>256</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>454</v>
@@ -2571,19 +2571,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>22</v>
@@ -2592,10 +2592,10 @@
         <v>22</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>257</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>259</v>
       </c>
@@ -2641,12 +2641,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>261</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>477</v>
@@ -2664,12 +2664,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>262</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>478</v>
@@ -2687,7 +2687,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>263</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>265</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>267</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>268</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>34</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>33</v>
@@ -2779,7 +2779,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>270</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>272</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>274</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>275</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>44</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>42</v>
@@ -2859,18 +2859,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>276</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>483</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>44</v>
@@ -2882,12 +2882,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>277</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>484</v>
@@ -2905,7 +2905,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="90" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>278</v>
       </c>
@@ -2913,10 +2913,10 @@
         <v>45</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>146</v>
@@ -2925,10 +2925,10 @@
         <v>47</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="75" x14ac:dyDescent="0.2">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>279</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>280</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>48</v>
@@ -2945,7 +2945,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>281</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>283</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>285</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>286</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>51</v>
@@ -2996,7 +2996,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>358</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>287</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>52</v>
@@ -3013,7 +3013,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>359</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>288</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>53</v>
@@ -3030,7 +3030,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="105" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>360</v>
       </c>
@@ -3038,16 +3038,16 @@
         <v>299</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>540</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>541</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>361</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>362</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>363</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>364</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>365</v>
       </c>
@@ -3132,15 +3132,15 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>366</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>61</v>
@@ -3158,12 +3158,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>367</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>486</v>
@@ -3181,12 +3181,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>368</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>487</v>
@@ -3204,7 +3204,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>369</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>370</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>371</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>372</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>304</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>69</v>
@@ -3287,7 +3287,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>373</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>291</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>491</v>
+        <v>601</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>70</v>
@@ -3304,7 +3304,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>374</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>73</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>71</v>
@@ -3321,7 +3321,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>375</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>305</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>74</v>
@@ -3344,7 +3344,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>376</v>
       </c>
@@ -3352,10 +3352,10 @@
         <v>292</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>73</v>
@@ -3367,7 +3367,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>377</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>306</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>75</v>
@@ -3387,7 +3387,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>378</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>78</v>
@@ -3407,17 +3407,17 @@
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="E48" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>379</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>466</v>
@@ -3435,15 +3435,15 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>380</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E50" s="10" t="s">
         <v>214</v>
@@ -3458,7 +3458,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>381</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>86</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>83</v>
@@ -3478,20 +3478,20 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C52" s="7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>382</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>85</v>
@@ -3506,18 +3506,18 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>383</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>467</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>59</v>
@@ -3529,15 +3529,15 @@
         <v>176</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="150" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>384</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>88</v>
@@ -3552,15 +3552,15 @@
         <v>177</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>385</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>89</v>
@@ -3575,7 +3575,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>386</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="165" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>387</v>
       </c>
@@ -3600,10 +3600,10 @@
         <v>307</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>25</v>
@@ -3615,7 +3615,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>388</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>308</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>91</v>
@@ -3638,7 +3638,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>389</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>309</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>215</v>
@@ -3661,7 +3661,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>390</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>310</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>216</v>
@@ -3684,7 +3684,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>391</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>311</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>93</v>
@@ -3707,15 +3707,15 @@
         <v>184</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>392</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>94</v>
@@ -3730,7 +3730,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>393</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>469</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>95</v>
@@ -3753,7 +3753,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>394</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>313</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>96</v>
@@ -3776,7 +3776,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="135" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>395</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>293</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>98</v>
@@ -3799,7 +3799,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>396</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>314</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>99</v>
@@ -3822,7 +3822,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>397</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>72</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>100</v>
@@ -3839,7 +3839,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>398</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
         <v>399</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>400</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>295</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>104</v>
@@ -3902,7 +3902,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>401</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>296</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>105</v>
@@ -3919,15 +3919,15 @@
         <v>194</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
         <v>402</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>107</v>
@@ -3942,15 +3942,15 @@
         <v>195</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
         <v>403</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>108</v>
@@ -3965,7 +3965,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
         <v>404</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
         <v>405</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>406</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>407</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>408</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>297</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>114</v>
@@ -4056,7 +4056,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
         <v>409</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>117</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E80" s="7" t="s">
         <v>116</v>
@@ -4073,7 +4073,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
         <v>410</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>317</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>118</v>
@@ -4096,7 +4096,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>411</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>318</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>119</v>
@@ -4119,7 +4119,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
         <v>412</v>
       </c>
@@ -4128,7 +4128,7 @@
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>120</v>
@@ -4143,7 +4143,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>413</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>320</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>121</v>
@@ -4166,7 +4166,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="120" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>414</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>415</v>
       </c>
@@ -4203,10 +4203,10 @@
         <v>298</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>25</v>
@@ -4218,7 +4218,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>125</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>416</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>322</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>127</v>
@@ -4243,7 +4243,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>419</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>323</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>128</v>
@@ -4260,7 +4260,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>420</v>
       </c>
@@ -4268,13 +4268,13 @@
         <v>324</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I90" s="5" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>421</v>
       </c>
@@ -4282,13 +4282,13 @@
         <v>325</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I91" s="5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>422</v>
       </c>
@@ -4296,13 +4296,13 @@
         <v>326</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I92" s="5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>423</v>
       </c>
@@ -4310,13 +4310,13 @@
         <v>327</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I93" s="5" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>424</v>
       </c>
@@ -4324,13 +4324,13 @@
         <v>328</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I94" s="5" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>425</v>
       </c>
@@ -4338,13 +4338,13 @@
         <v>329</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I95" s="5" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>426</v>
       </c>
@@ -4352,13 +4352,13 @@
         <v>330</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I96" s="5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
         <v>427</v>
       </c>
@@ -4366,13 +4366,13 @@
         <v>331</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I97" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
         <v>428</v>
       </c>
@@ -4380,13 +4380,13 @@
         <v>332</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I98" s="5" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
         <v>429</v>
       </c>
@@ -4394,13 +4394,13 @@
         <v>333</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I99" s="5" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>430</v>
       </c>
@@ -4408,13 +4408,13 @@
         <v>334</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I100" s="5" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
         <v>431</v>
       </c>
@@ -4422,13 +4422,13 @@
         <v>335</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I101" s="5" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
         <v>432</v>
       </c>
@@ -4436,13 +4436,13 @@
         <v>336</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I102" s="5" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
         <v>433</v>
       </c>
@@ -4450,13 +4450,13 @@
         <v>337</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I103" s="5" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>434</v>
       </c>
@@ -4464,13 +4464,13 @@
         <v>338</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I104" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
         <v>435</v>
       </c>
@@ -4478,13 +4478,13 @@
         <v>339</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I105" s="5" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
         <v>436</v>
       </c>
@@ -4492,13 +4492,13 @@
         <v>340</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I106" s="5" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
         <v>418</v>
       </c>
@@ -4506,13 +4506,13 @@
         <v>341</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I107" s="5" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
         <v>417</v>
       </c>
@@ -4520,13 +4520,13 @@
         <v>342</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I108" s="5" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
         <v>437</v>
       </c>
@@ -4534,13 +4534,13 @@
         <v>343</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I109" s="5" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
         <v>438</v>
       </c>
@@ -4548,13 +4548,13 @@
         <v>344</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I110" s="5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
         <v>439</v>
       </c>
@@ -4562,13 +4562,13 @@
         <v>345</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I111" s="5" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
         <v>440</v>
       </c>
@@ -4576,13 +4576,13 @@
         <v>346</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I112" s="5" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
         <v>441</v>
       </c>
@@ -4590,13 +4590,13 @@
         <v>347</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I113" s="5" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
         <v>442</v>
       </c>
@@ -4604,13 +4604,13 @@
         <v>348</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I114" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
         <v>443</v>
       </c>
@@ -4618,13 +4618,13 @@
         <v>349</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I115" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
         <v>444</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>350</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H116" s="5" t="s">
         <v>84</v>
@@ -4641,7 +4641,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
         <v>445</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>351</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H117" s="5" t="s">
         <v>84</v>
@@ -4658,7 +4658,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
         <v>446</v>
       </c>
@@ -4666,13 +4666,13 @@
         <v>352</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I118" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
         <v>447</v>
       </c>
@@ -4680,13 +4680,13 @@
         <v>353</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I119" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>448</v>
       </c>
@@ -4694,13 +4694,13 @@
         <v>354</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I120" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
         <v>449</v>
       </c>
@@ -4708,13 +4708,13 @@
         <v>355</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I121" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
         <v>450</v>
       </c>
@@ -4722,13 +4722,13 @@
         <v>356</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I122" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
         <v>451</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>357</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I123" s="5" t="s">
         <v>251</v>

</xml_diff>